<commit_message>
Turned on the Stage-1 of MSR creator. For the first time run, this stage must be executed otherwise, the code will not have the starting spatial files for creating the MSR regions.
</commit_message>
<xml_diff>
--- a/1. MSR Creator/ControlFile_MSRCreator.xlsx
+++ b/1. MSR Creator/ControlFile_MSRCreator.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BHussain\Dropbox (IRENA)\01 My work folder\2. MSR\20210105 zoning codes\2. MSR_OpenRepo\1. MSR Creator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://irena-my.sharepoint.com/personal/bhussain_irena_org/Documents/01 My work folder/2. MSR/20210105 zoning codes/2. Model-Supply-Regions-MSR-Toolset/1. MSR Creator/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_C3E42DC95BC4978368CAB72B79A5ABDC9CA1094B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10AA41CB-2254-4691-A6CB-3B075F2717D6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="21480" yWindow="-8625" windowWidth="19440" windowHeight="10320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paths" sheetId="9" r:id="rId1"/>
@@ -26,15 +27,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -522,7 +514,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -611,9 +603,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -894,7 +885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -904,14 +895,14 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.36328125" customWidth="1"/>
-    <col min="3" max="3" width="39.26953125" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>128</v>
       </c>
@@ -922,7 +913,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>129</v>
       </c>
@@ -933,7 +924,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>131</v>
       </c>
@@ -944,7 +935,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>132</v>
       </c>
@@ -955,7 +946,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>133</v>
       </c>
@@ -972,23 +963,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83.453125" customWidth="1"/>
-    <col min="3" max="3" width="69.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.42578125" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>128</v>
       </c>
@@ -999,7 +990,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>135</v>
       </c>
@@ -1010,7 +1001,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>136</v>
       </c>
@@ -1021,7 +1012,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>144</v>
       </c>
@@ -1032,7 +1023,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>138</v>
       </c>
@@ -1043,7 +1034,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>137</v>
       </c>
@@ -1054,7 +1045,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>139</v>
       </c>
@@ -1065,7 +1056,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>140</v>
       </c>
@@ -1076,18 +1067,18 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>102</v>
       </c>
@@ -1098,7 +1089,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>98</v>
       </c>
@@ -1109,7 +1100,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>99</v>
       </c>
@@ -1127,7 +1118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1137,14 +1128,14 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1796875" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>128</v>
       </c>
@@ -1153,7 +1144,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
@@ -1161,7 +1152,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>107</v>
       </c>
@@ -1169,7 +1160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>108</v>
       </c>
@@ -1177,7 +1168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>109</v>
       </c>
@@ -1185,7 +1176,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>110</v>
       </c>
@@ -1193,7 +1184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>111</v>
       </c>
@@ -1201,7 +1192,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>112</v>
       </c>
@@ -1209,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>113</v>
       </c>
@@ -1217,7 +1208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>117</v>
       </c>
@@ -1225,7 +1216,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>114</v>
       </c>
@@ -1233,7 +1224,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>115</v>
       </c>
@@ -1241,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>116</v>
       </c>
@@ -1249,7 +1240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>145</v>
       </c>
@@ -1257,7 +1248,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>120</v>
       </c>
@@ -1265,7 +1256,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>119</v>
       </c>
@@ -1273,7 +1264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>118</v>
       </c>
@@ -1283,7 +1274,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -1293,7 +1284,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1303,25 +1294,25 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -1332,7 +1323,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -1343,7 +1334,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1354,7 +1345,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -1365,7 +1356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1376,7 +1367,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1387,7 +1378,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
@@ -1398,7 +1389,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
@@ -1409,7 +1400,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -1431,7 +1422,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
@@ -1442,7 +1433,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>59</v>
       </c>
@@ -1453,7 +1444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1464,7 +1455,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1475,7 +1466,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
@@ -1486,7 +1477,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>53</v>
       </c>
@@ -1497,7 +1488,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -1508,7 +1499,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -1519,7 +1510,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -1530,7 +1521,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>56</v>
       </c>
@@ -1541,7 +1532,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>26</v>
       </c>
@@ -1552,7 +1543,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +1554,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
@@ -1574,7 +1565,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>52</v>
       </c>
@@ -1585,7 +1576,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>29</v>
       </c>
@@ -1596,7 +1587,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1607,7 +1598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1618,7 +1609,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1629,7 +1620,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>57</v>
       </c>
@@ -1640,7 +1631,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>33</v>
       </c>
@@ -1651,7 +1642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>34</v>
       </c>
@@ -1662,7 +1653,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>35</v>
       </c>
@@ -1673,7 +1664,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>36</v>
       </c>
@@ -1684,7 +1675,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>37</v>
       </c>
@@ -1695,7 +1686,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>38</v>
       </c>
@@ -1706,7 +1697,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>39</v>
       </c>
@@ -1717,7 +1708,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>40</v>
       </c>
@@ -1728,7 +1719,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>41</v>
       </c>
@@ -1739,7 +1730,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>54</v>
       </c>
@@ -1750,7 +1741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>42</v>
       </c>
@@ -1761,7 +1752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>43</v>
       </c>
@@ -1772,7 +1763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>55</v>
       </c>
@@ -1783,7 +1774,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -1794,7 +1785,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -1805,7 +1796,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1816,7 +1807,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -1827,7 +1818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
@@ -1838,7 +1829,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -1849,7 +1840,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>60</v>
       </c>
@@ -1860,7 +1851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>61</v>
       </c>
@@ -1871,7 +1862,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>50</v>
       </c>
@@ -1882,7 +1873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
@@ -1893,7 +1884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>63</v>
       </c>
@@ -1904,7 +1895,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>64</v>
       </c>
@@ -1915,7 +1906,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>66</v>
       </c>
@@ -1926,7 +1917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>67</v>
       </c>
@@ -1937,7 +1928,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>68</v>
       </c>
@@ -1949,8 +1940,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B53">
-    <sortState ref="A2:B53">
+  <autoFilter ref="A1:B53" xr:uid="{00000000-0009-0000-0000-000003000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B53">
       <sortCondition ref="A1:A53"/>
     </sortState>
   </autoFilter>
@@ -1959,7 +1950,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1969,25 +1960,25 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.54296875" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>72</v>
       </c>
@@ -1998,7 +1989,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>73</v>
       </c>
@@ -2009,7 +2000,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>74</v>
       </c>
@@ -2020,7 +2011,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>75</v>
       </c>
@@ -2031,7 +2022,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>76</v>
       </c>
@@ -2042,7 +2033,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>77</v>
       </c>
@@ -2053,7 +2044,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>78</v>
       </c>
@@ -2064,7 +2055,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>79</v>
       </c>
@@ -2075,7 +2066,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>80</v>
       </c>
@@ -2086,7 +2077,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>81</v>
       </c>
@@ -2097,7 +2088,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>88</v>
       </c>
@@ -2108,7 +2099,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>89</v>
       </c>
@@ -2119,7 +2110,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>90</v>
       </c>
@@ -2130,7 +2121,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>91</v>
       </c>
@@ -2141,7 +2132,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>103</v>
       </c>
@@ -2152,7 +2143,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>104</v>
       </c>
@@ -2163,7 +2154,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>126</v>
       </c>
@@ -2174,11 +2165,11 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="9">
         <v>1960000</v>
       </c>
       <c r="C19" s="6" t="s">

</xml_diff>